<commit_message>
Timesheet updated by sruthi
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet (2).xlsx
+++ b/Process/Timesheet/PTW-Timesheet (2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5907952D-29DF-46A9-8ADF-64FA8C56F4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DFDAA1D-C457-4EF2-94A2-40BA9CB5A695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="22-04-22" sheetId="55" r:id="rId14"/>
     <sheet name="23-04-22" sheetId="56" r:id="rId15"/>
     <sheet name="25-04-22" sheetId="57" r:id="rId16"/>
+    <sheet name="26-04-22" sheetId="58" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="492">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1506,20 +1507,230 @@
     <t>Lunch break - 1:30 mins</t>
   </si>
   <si>
-    <t>Team meeting-20 mins, meeting with client -23 mins,Team meeting(For layout)</t>
+    <t xml:space="preserve">Trainee Feedback layout ,Course Feedback layout </t>
+  </si>
+  <si>
+    <t>Team meeting-20 mins, meeting with client -23 mins,Team meeting( About layout completion)-30 min, working on layout for trainee feedback and course feedback -3h30mins</t>
   </si>
   <si>
     <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service - 4hrs</t>
   </si>
   <si>
     <t>lunch and breaks - 90mins</t>
+  </si>
+  <si>
+    <t>Web Api services</t>
+  </si>
+  <si>
+    <t>8:30 - 9:05(35mins) : Updating timesheet and MOM,
+9:05 - 9:30(25mins) : Team meeting,      
+9:30 - 10:20(50mins) : Softskill,
+10:20 - 10:40(20mins) : break,
+10:45 - 11:45(60mins) : Web api services added(User,Department,Role),  
+11:45 - 12:15(30mins) : Estimation of pages in TMS, 
+12:15 - 12:25(10mins) : Helping in resolve a conflict,
+12:35 - 12:55(20mins) : Client meeting,
+1:00 - 1:40(40mins) : Lunch,
+2:00 - 2:40(40mins) : Web api session among team,  
+2:40 - 3:00(10mins) : worked on a Services,  
+3:00 - 3:40(40mins) : rework on a new repository,                                        
+3:40 - 4:15(35mins) : Implementing Serilog in api,
+4:15 - 4:30(15mins) : break,
+4:30 - 5:15(45mins) : Resolving conflict in webapi,
+5:15 - 5:45(30mins) : Clarifying about repository and worked on new repository
+7:00 - 7:45(45mis) : Midlleware exploration</t>
+  </si>
+  <si>
+    <t>6.3 hrs</t>
+  </si>
+  <si>
+    <t>3.10 hrs</t>
+  </si>
+  <si>
+    <t>Web api (Debugging Errors-(8:15-9:00),                    repository(9:00-9:44),(10:40-12:00) ,                                 Estimation and discussion(12:00-12-33),Meeting with Rafi(12:36-12:52),Timesheet update(2:00-2:15),</t>
+  </si>
+  <si>
+    <t>Softskill session(9:44-10:33),Break(1:05-1:40),sending mail for installation(2:40-2:45),Webapi exploring(3:00-3:30),college call(3:30-3:45),Break(3:45-4:00),System installation (4:00-4:25),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Api exploration,
+Ef Core exploration
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00 - 9:20 : TimeSheet,
+9:20 - 9:35 : Team meeting,      
+9:35 - 10:20 : Softskill,
+10:20 - 10:40 : Break,   
+10:40 - 10:55 : Estimation explaination,
+10:55 - 11:45 : Web api services added(DbContext,Migrations,UserService), 
+11:45 - 12:35 : Estimation of pages in TMS, 
+12:35 - 12:56 : Client meeting,
+12:56 - 1:30 : Lunch
+1:30 - 2:00 : preparing for web api session 
+2:00 - 3:00 : worked on UserServices.cs,
+3:00 - 4:00 : Web api session among team,                                         
+4:00 - 4:30 : worked on IRepository.cs,
+4:30 - 4:45 : Break,
+4:45 - 5:30 : Resolving conflict in Webapi </t>
+  </si>
+  <si>
+    <t>Component in angular for common Layout pages</t>
+  </si>
+  <si>
+    <t>8.40-9.00   : Updating Timesheet
+9.05-9.30   : Team Discussion about work Progress
+10.40-12.30 : Layout Integration and corrections in Layout
+12.35-12.56 : Client(Rafi) Meeting
+2.00-2.20   : Uploading Layout pages as static pages to Git publish
+2.20-2.50   : Identify the Unique and Common Layout pages for Estimation
+3.00-4.00   : Web Api Session amoung Team
+4.30-4.50   : Presenting the Layout to the Client(Rafi)
+4.50-5.00   : Discussion with Layout team about changes in Layout
+5.00-5.40   : Discussion about Layout page Estimation</t>
+  </si>
+  <si>
+    <t>9.30-10.20  : Softskill session
+10.20-10.40 : Tea Break
+1.00-2.00   : Lunch Break
+4.00-4.30   : Tea Break</t>
+  </si>
+  <si>
+    <t>Estimation and Layout Correction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Updating Timesheet and HLD Document
+9:05 - 9:30 : Team meeting
+10:40-10:55 : Estimation explanation meeting
+11:00-11:30 : Integrating my MOM layout with other layout pages 
+11.30-12.15: Helping in Attendence Layout
+12:35 - 12:56 : meeting with Rafi 
+2.00-3.00 mins : Identifying the pages and Estimation
+4.35-4.50 : EF Session with other team 
+4.55-5.45: Layout Correction Explanation and Estimation
+</t>
+  </si>
+  <si>
+    <t>9:30 - 10:20 : Softskill
+3:00 - 4:00: webAPI Session with team
+10:20 - 10:40 : break
+1:00 - 1:40 : Lunch
+4:00- 4:15 : break</t>
+  </si>
+  <si>
+    <t>Refining the layout and responvise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.05 : Updating Timesheet 
+9:05 - 9:30 : Team meeting
+12:35 - 12:56 : meeting with Rafi 
+2.00-3.00 : Identifying the Unique page for Estimation
+4.35-4.50 : Web API Session with team 
+4.55-5.30: Layout Correction Explanation and Estimation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+9.30-10.30 : Soft skill
+10.30-11.45: prepare for internal review
+1-1.45-Lunch
+3.55-4.10-Break
+5.30-6:Internal Review with Anitha
+</t>
+  </si>
+  <si>
+    <t>Layout page for Assign course and Create topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:20-9:30-Team meeting,
+10:40-12:30:Worked on Layout page (Assign course and create topic),
+12:35-12:55:Meeting with Rafi,
+2:00-3:00: Web Api session among team,
+4:30-5:30-Layout corrections and responsivenss 
+</t>
+  </si>
+  <si>
+    <t>9:30-10:20:Softskill session,
+10:20-10:40:Break,
+1:00-1:50:lunch break,
+3:00-4:00:Explored about entity framework,
+4:00-4:20:Tea break,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Updating Timesheet 
+9:05 - 9:30 : Team meeting
+9:30 - 10:20 : Softskill session(Problem Solving)
+10:20 - 10:40 : break
+10:40-10:55 : Estimation explanation meeting
+11.00-12.30: worked on attendace layout
+12:35 - 12:56 : meeting with Rafi 
+1:00 - 1:40 : Lunch
+2:00 - 3:00: webAPI Session with team members
+3.00-3.20:uploading files in github
+4:30- 4:45 : break
+4.45-5.45:Exploration on web api
+7.00-8.00:Brushing up of basic concepts in c#
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     3 hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                                     5 hrs</t>
+  </si>
+  <si>
+    <t>8.40-9.00   : Updating Timesheet
+9.05-9.30   : Team Discussion about work Progress
+10.40-12.30 : intergarting the layout (TMS layout)
+12.35-12.56 : Client(Rafi) Meeting
+2.00-2.20   : creating the repositiers
+2.20-2.50   : Identify the Unique and Common Layout pages for Estimation
+3.00-4.00   : Web Api Session amoung Team
+4.30-4.50   : Presenting the Layout to the Client(Rafi)
+4.50-5.00   : Discussion with Layout team about changes in Layout
+5.00-5.40   : Discussion about Layout page Estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Refining course feedback layout
+9:05 - 9:30 : Team meeting
+9:30 - 10:20(50mins) : Softskill,10:40-10:55 : Estimation explanation meeting
+11:00-11:30 : Integrating my MOM layout with other layout pages 
+11.30-12.15: Helping in Attendence Layout
+12:35 - 12:56 : meeting with Rafi 
+2.00-3.00 mins : Identifying the pages and Estimation
+4.35-4.50 : Web API Session with other team 
+4.55-5.45: Layout Correction Explanation and Estimation
+</t>
+  </si>
+  <si>
+    <t>Estimation for TMS and refineed layouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Updating Timesheet and HLD Document
+9:05 - 9:30 : Team meeting for work status
+10:40-10:55 : Estimation explanation meeting with team
+11:00-11:45 : Refining schedule review and review layout for TMS 
+11:45-12:30 : reviewing others layouts
+12:35 - 12:56 : meeting with client 
+2:00-3:00 : Identifying the pages for Estimation
+4.55-5.45: Layout Correction Explanation and Estimation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:30 - 10:20 : Softskill session
+10:20 - 10:40 : break
+1:00 - 1:40 : Lunch break
+3:00 - 4:00: Web API Session with team members
+4:00- 4:20 : break
+4.35-4.50 : Entity framework Session with other team </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1656,6 +1867,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1665,7 +1883,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1756,12 +1974,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1885,6 +2118,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1894,6 +2136,96 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1903,32 +2235,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3145,14 +3456,14 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
@@ -3263,7 +3574,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="51">
+    <row r="9" spans="1:10" ht="37.5">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
@@ -3356,7 +3667,7 @@
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3379,7 +3690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63.75">
+    <row r="2" spans="1:7" ht="74.25">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -3455,7 +3766,7 @@
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" ht="51">
+    <row r="6" spans="1:7" ht="49.5">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
@@ -3474,7 +3785,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="51">
+    <row r="7" spans="1:7" ht="49.5">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
@@ -3531,7 +3842,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="89.25">
+    <row r="10" spans="1:7" ht="61.5">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -3597,8 +3908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2D3FBA-C93D-4333-B7E1-C7BA11A34680}">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="J5" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15"/>
@@ -3607,7 +3918,7 @@
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30">
+    <row r="1" spans="1:22">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3656,14 +3967,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="78" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:22" ht="101.25" customHeight="1">
       <c r="A4" s="16" t="s">
@@ -3775,7 +4086,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:22" ht="38.25">
+    <row r="10" spans="1:22" ht="25.5">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -3848,7 +4159,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3862,7 +4173,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3906,16 +4217,16 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="78" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
-    </row>
-    <row r="4" spans="1:7" ht="51">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
+    </row>
+    <row r="4" spans="1:7" ht="49.5">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
@@ -4023,27 +4334,27 @@
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="81" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="59"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="83"/>
     </row>
     <row r="11" spans="1:7" ht="36.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="81" t="s">
         <v>298</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="59"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="83"/>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4076,8 +4387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14287F61-8AE3-4555-BA8D-07210E8D9156}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4091,7 +4402,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -4114,7 +4425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63.75">
+    <row r="2" spans="1:7" ht="61.5">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -4135,10 +4446,10 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="50" t="s">
         <v>438</v>
       </c>
       <c r="D3" s="43"/>
@@ -4154,7 +4465,7 @@
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="48" t="s">
         <v>319</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -4260,37 +4571,40 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="35.25" customHeight="1">
+    <row r="10" spans="1:7" ht="55.5" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="45" t="s">
         <v>456</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="53" t="s">
         <v>457</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="35" t="s">
         <v>458</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>459</v>
       </c>
-      <c r="G10" s="50"/>
-    </row>
-    <row r="11" spans="1:7" ht="35.25" customHeight="1">
+      <c r="G10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="79.5" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="52" t="s">
         <v>460</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="51" t="s">
+        <v>461</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4302,14 +4616,253 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7172FC-5606-4FD6-B7B3-02AB5BD496A0}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="56" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="267" customHeight="1">
+      <c r="A2" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>464</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>465</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
+        <v>466</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>467</v>
+      </c>
+      <c r="G2" s="71"/>
+    </row>
+    <row r="3" spans="1:7" ht="147.75" customHeight="1">
+      <c r="A3" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59" t="s">
+        <v>468</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>469</v>
+      </c>
+      <c r="G3" s="72"/>
+    </row>
+    <row r="4" spans="1:7" ht="244.5" customHeight="1">
+      <c r="A4" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>351</v>
+      </c>
+      <c r="G4" s="55"/>
+    </row>
+    <row r="5" spans="1:7" ht="228.75" customHeight="1">
+      <c r="A5" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>472</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58" t="s">
+        <v>473</v>
+      </c>
+      <c r="F5" s="85" t="s">
+        <v>474</v>
+      </c>
+      <c r="G5" s="54"/>
+    </row>
+    <row r="6" spans="1:7" ht="120" customHeight="1">
+      <c r="A6" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="58" t="s">
+        <v>475</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="64" t="s">
+        <v>476</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>477</v>
+      </c>
+      <c r="G6" s="73"/>
+    </row>
+    <row r="7" spans="1:7" ht="132.75" customHeight="1">
+      <c r="A7" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58" t="s">
+        <v>478</v>
+      </c>
+      <c r="D7" s="58"/>
+      <c r="E7" s="64" t="s">
+        <v>479</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>480</v>
+      </c>
+      <c r="G7" s="71"/>
+    </row>
+    <row r="8" spans="1:7" ht="150" customHeight="1">
+      <c r="A8" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="65"/>
+      <c r="C8" s="84" t="s">
+        <v>481</v>
+      </c>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59" t="s">
+        <v>482</v>
+      </c>
+      <c r="F8" s="65" t="s">
+        <v>483</v>
+      </c>
+      <c r="G8" s="71"/>
+    </row>
+    <row r="9" spans="1:7" ht="230.25" customHeight="1">
+      <c r="A9" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>484</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>486</v>
+      </c>
+      <c r="G9" s="71"/>
+    </row>
+    <row r="10" spans="1:7" ht="172.5" customHeight="1">
+      <c r="A10" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58" t="s">
+        <v>430</v>
+      </c>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58" t="s">
+        <v>487</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>374</v>
+      </c>
+      <c r="G10" s="71"/>
+    </row>
+    <row r="11" spans="1:7" ht="189.75" customHeight="1">
+      <c r="A11" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="66"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="64" t="s">
+        <v>488</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="141.75" customHeight="1">
+      <c r="A12" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67" t="s">
+        <v>489</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="68" t="s">
+        <v>490</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>491</v>
+      </c>
+      <c r="G12" s="74"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>